<commit_message>
macro support for excel wrapper with tests
</commit_message>
<xml_diff>
--- a/excel_wrapper/test/excel_wrapper_test.xlsx
+++ b/excel_wrapper/test/excel_wrapper_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\excel_wrapper_meta\excel_wrapper\src\excel_wrapper\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\excel_wrapper_meta\excel_wrapper\excel_wrapper\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,17 +19,19 @@
   <definedNames>
     <definedName name="b">Sheet1!$B$3</definedName>
     <definedName name="bout">Sheet1!$F$3</definedName>
+    <definedName name="macroVar_in">Sheet1!$B$7</definedName>
+    <definedName name="macroVar_out">Sheet1!$F$7</definedName>
     <definedName name="s">Sheet1!$B$4</definedName>
     <definedName name="sout">Sheet1!$F$4</definedName>
     <definedName name="x">Sheet1!$B$2</definedName>
     <definedName name="y">Sheet1!$F$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Inputs</t>
   </si>
@@ -74,12 +76,15 @@
   </si>
   <si>
     <t>Hello</t>
+  </si>
+  <si>
+    <t>kl.;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -485,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,6 +581,14 @@
         <v>0.12</v>
       </c>
       <c r="D5" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>